<commit_message>
:pushpin:Finish the exp of 变长指令周期---时序发生器FSM设计
</commit_message>
<xml_diff>
--- a/7.单总线CPU/单总线实验资料包(愚人节版)/1.单总线MIPS三级时序产生器逻辑自动生成(2020-4-1).xlsx
+++ b/7.单总线CPU/单总线实验资料包(愚人节版)/1.单总线MIPS三级时序产生器逻辑自动生成(2020-4-1).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\迅雷下载\计算机硬件系统设计\单总线CPU\单总线实验资料包(愚人节版)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Computer_Orgnization_and_Architecture\hustzc\Make_A_CPU_Youself\7.单总线CPU\单总线实验资料包(愚人节版)\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C995F82A-9B47-48EF-9AD3-DD3AA34F691A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12465" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="状态转换表" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">输出函数自动生成!$A$1:$L$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">状态转换表!$O$2:$R$22</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -170,7 +181,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
@@ -1682,15 +1693,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W20" sqref="W20"/>
+      <selection pane="bottomLeft" activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1979,111 +1990,125 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B7" s="28" t="str">
+      <c r="A7" s="28">
+        <f>IF(ISNUMBER($E7),IF(MOD($E7,16)/8&gt;=1,1,0),"")</f>
+        <v>0</v>
+      </c>
+      <c r="B7" s="28">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C7" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="C7" s="28">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D7" s="29" t="str">
+        <v>1</v>
+      </c>
+      <c r="D7" s="29">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E7" s="77"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="77">
+        <v>3</v>
+      </c>
       <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
+      <c r="G7" s="42">
+        <v>1</v>
+      </c>
       <c r="H7" s="42"/>
       <c r="I7" s="42"/>
       <c r="J7" s="42"/>
       <c r="K7" s="67"/>
       <c r="L7" s="42"/>
       <c r="M7" s="67"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="28" t="str">
+      <c r="N7" s="78">
+        <v>4</v>
+      </c>
+      <c r="O7" s="28">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P7" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="P7" s="28">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q7" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="28">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R7" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="R7" s="29">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B8" s="33" t="str">
+      <c r="A8" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B8" s="33">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C8" s="33" t="str">
+        <v>0</v>
+      </c>
+      <c r="C8" s="33">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D8" s="34" t="str">
+        <v>1</v>
+      </c>
+      <c r="D8" s="34">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E8" s="35"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="35">
+        <v>3</v>
+      </c>
       <c r="F8" s="36"/>
       <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
+      <c r="H8" s="37">
+        <v>1</v>
+      </c>
       <c r="I8" s="37"/>
       <c r="J8" s="37"/>
       <c r="K8" s="40"/>
       <c r="L8" s="37"/>
       <c r="M8" s="40"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="33" t="str">
+      <c r="N8" s="66">
+        <v>4</v>
+      </c>
+      <c r="O8" s="33">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P8" s="33" t="str">
+        <v>0</v>
+      </c>
+      <c r="P8" s="33">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q8" s="33" t="str">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="33">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R8" s="34" t="str">
+        <v>0</v>
+      </c>
+      <c r="R8" s="34">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B9" s="28" t="str">
+      <c r="A9" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B9" s="28">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C9" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="C9" s="28">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D9" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="D9" s="29">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E9" s="77"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="77">
+        <v>4</v>
+      </c>
       <c r="F9" s="41"/>
       <c r="G9" s="42"/>
       <c r="H9" s="42"/>
@@ -2092,42 +2117,46 @@
       <c r="K9" s="67"/>
       <c r="L9" s="42"/>
       <c r="M9" s="67"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="28" t="str">
+      <c r="N9" s="78">
+        <v>5</v>
+      </c>
+      <c r="O9" s="28">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P9" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="P9" s="28">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q9" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="28">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R9" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="R9" s="29">
         <f t="shared" si="7"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B10" s="33" t="str">
+      <c r="A10" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="33">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C10" s="33" t="str">
+        <v>1</v>
+      </c>
+      <c r="C10" s="33">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D10" s="34" t="str">
+        <v>0</v>
+      </c>
+      <c r="D10" s="34">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E10" s="35"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="35">
+        <v>5</v>
+      </c>
       <c r="F10" s="36"/>
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
@@ -2136,86 +2165,96 @@
       <c r="K10" s="40"/>
       <c r="L10" s="37"/>
       <c r="M10" s="40"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="33" t="str">
+      <c r="N10" s="66">
+        <v>6</v>
+      </c>
+      <c r="O10" s="33">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P10" s="33" t="str">
+        <v>0</v>
+      </c>
+      <c r="P10" s="33">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q10" s="33" t="str">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="33">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R10" s="34" t="str">
+        <v>1</v>
+      </c>
+      <c r="R10" s="34">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B11" s="28" t="str">
+      <c r="A11" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B11" s="28">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C11" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="C11" s="28">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D11" s="29" t="str">
+        <v>1</v>
+      </c>
+      <c r="D11" s="29">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E11" s="77"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="77">
+        <v>3</v>
+      </c>
       <c r="F11" s="41"/>
       <c r="G11" s="42"/>
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
+      <c r="J11" s="42">
+        <v>1</v>
+      </c>
       <c r="K11" s="67"/>
       <c r="L11" s="42"/>
       <c r="M11" s="67"/>
-      <c r="N11" s="78"/>
-      <c r="O11" s="28" t="str">
+      <c r="N11" s="78">
+        <v>6</v>
+      </c>
+      <c r="O11" s="28">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P11" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="P11" s="28">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q11" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="28">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R11" s="29" t="str">
+        <v>1</v>
+      </c>
+      <c r="R11" s="29">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B12" s="33" t="str">
+      <c r="A12" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B12" s="33">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C12" s="33" t="str">
+        <v>1</v>
+      </c>
+      <c r="C12" s="33">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D12" s="34" t="str">
+        <v>1</v>
+      </c>
+      <c r="D12" s="34">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E12" s="35"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="35">
+        <v>6</v>
+      </c>
       <c r="F12" s="36"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
@@ -2224,42 +2263,46 @@
       <c r="K12" s="40"/>
       <c r="L12" s="37"/>
       <c r="M12" s="40"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="33" t="str">
+      <c r="N12" s="66">
+        <v>7</v>
+      </c>
+      <c r="O12" s="33">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P12" s="33" t="str">
+        <v>0</v>
+      </c>
+      <c r="P12" s="33">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q12" s="33" t="str">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="33">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R12" s="34" t="str">
+        <v>1</v>
+      </c>
+      <c r="R12" s="34">
         <f t="shared" si="7"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B13" s="28" t="str">
+      <c r="A13" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B13" s="28">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C13" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="C13" s="28">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D13" s="29" t="str">
+        <v>1</v>
+      </c>
+      <c r="D13" s="29">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E13" s="77"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="77">
+        <v>7</v>
+      </c>
       <c r="F13" s="41"/>
       <c r="G13" s="42"/>
       <c r="H13" s="42"/>
@@ -2268,42 +2311,46 @@
       <c r="K13" s="67"/>
       <c r="L13" s="42"/>
       <c r="M13" s="67"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="28" t="str">
+      <c r="N13" s="78">
+        <v>8</v>
+      </c>
+      <c r="O13" s="28">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P13" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="P13" s="28">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q13" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="28">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R13" s="29" t="str">
+        <v>0</v>
+      </c>
+      <c r="R13" s="29">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B14" s="33" t="str">
+      <c r="A14" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B14" s="33">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C14" s="33" t="str">
+        <v>0</v>
+      </c>
+      <c r="C14" s="33">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D14" s="34" t="str">
+        <v>0</v>
+      </c>
+      <c r="D14" s="34">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E14" s="35"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="35">
+        <v>8</v>
+      </c>
       <c r="F14" s="36"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
@@ -2312,110 +2359,132 @@
       <c r="K14" s="37"/>
       <c r="L14" s="37"/>
       <c r="M14" s="40"/>
-      <c r="N14" s="66"/>
-      <c r="O14" s="33" t="str">
+      <c r="N14" s="66">
+        <v>0</v>
+      </c>
+      <c r="O14" s="33">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P14" s="33" t="str">
+        <v>0</v>
+      </c>
+      <c r="P14" s="33">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q14" s="33" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="33">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R14" s="34" t="str">
+        <v>0</v>
+      </c>
+      <c r="R14" s="34">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B15" s="28" t="str">
+      <c r="A15" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B15" s="28">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C15" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="C15" s="28">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D15" s="29" t="str">
+        <v>1</v>
+      </c>
+      <c r="D15" s="29">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E15" s="77"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="77">
+        <v>3</v>
+      </c>
+      <c r="F15" s="41">
+        <v>0</v>
+      </c>
+      <c r="G15" s="42">
+        <v>0</v>
+      </c>
+      <c r="H15" s="42">
+        <v>0</v>
+      </c>
+      <c r="I15" s="42">
+        <v>0</v>
+      </c>
+      <c r="J15" s="42">
+        <v>0</v>
+      </c>
       <c r="K15" s="67"/>
       <c r="L15" s="42"/>
       <c r="M15" s="67"/>
-      <c r="N15" s="78"/>
-      <c r="O15" s="28" t="str">
+      <c r="N15" s="78">
+        <v>6</v>
+      </c>
+      <c r="O15" s="28">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P15" s="28" t="str">
+        <v>0</v>
+      </c>
+      <c r="P15" s="28">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q15" s="28" t="str">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="28">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R15" s="29" t="str">
+        <v>1</v>
+      </c>
+      <c r="R15" s="29">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B16" s="33" t="str">
+      <c r="A16" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B16" s="33">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C16" s="33" t="str">
+        <v>0</v>
+      </c>
+      <c r="C16" s="33">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="D16" s="34" t="str">
+        <v>1</v>
+      </c>
+      <c r="D16" s="34">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E16" s="35"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="35">
+        <v>3</v>
+      </c>
       <c r="F16" s="36"/>
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
+      <c r="J16" s="37">
+        <v>1</v>
+      </c>
       <c r="K16" s="37"/>
       <c r="L16" s="37"/>
       <c r="M16" s="40"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="33" t="str">
+      <c r="N16" s="66">
+        <v>6</v>
+      </c>
+      <c r="O16" s="33">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="P16" s="33" t="str">
+        <v>0</v>
+      </c>
+      <c r="P16" s="33">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q16" s="33" t="str">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="33">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="R16" s="34" t="str">
+        <v>1</v>
+      </c>
+      <c r="R16" s="34">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.2">
@@ -3135,14 +3204,14 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="616" yWindow="502" count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态机现态二进制" prompt="状态机现态二进制表示，由前列计算得到" sqref="A1 A32:C1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态变化控制信号" prompt="决定状态机迁移，如无关填“X”，输入信号名默认为Cx，可自行更改为和logisim自动生成电路的输入信号标签名一致！" sqref="F32:F1048576 G33:M1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态机现态" prompt="状态机现态" sqref="D32:D1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="现态10进制" prompt="现态10进制，方便大家输入，输入十进制后会自动计算二进制S3S2S1S0" sqref="E2:E31"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态输出" prompt="次态二进制表示，由前列10进制自动计算，不可修改" sqref="O2:R1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态10进制" prompt="次态10进制，方便大家输入，输入十进制后会自动计算二进制N3N2N1N0" sqref="N1:N1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态变化控制信号" prompt="决定状态机迁移，只填0或1，无关不填或填“X”，输入信号名默认为In#x，可自行更改为和logisim自动生成电路的输入信号标签名一致！" sqref="F1:M31"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="现态二进制" prompt="由现态十进制列自动计算得到，无需修改" sqref="A2:D31"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态机现态二进制" prompt="状态机现态二进制表示，由前列计算得到" sqref="A1 A32:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态变化控制信号" prompt="决定状态机迁移，如无关填“X”，输入信号名默认为Cx，可自行更改为和logisim自动生成电路的输入信号标签名一致！" sqref="F32:F1048576 G33:M1048576" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态机现态" prompt="状态机现态" sqref="D32:D1048576" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="现态10进制" prompt="现态10进制，方便大家输入，输入十进制后会自动计算二进制S3S2S1S0" sqref="E2:E31" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态输出" prompt="次态二进制表示，由前列10进制自动计算，不可修改" sqref="O2:R1048576" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态10进制" prompt="次态10进制，方便大家输入，输入十进制后会自动计算二进制N3N2N1N0" sqref="N1:N1048576" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态变化控制信号" prompt="决定状态机迁移，只填0或1，无关不填或填“X”，输入信号名默认为In#x，可自行更改为和logisim自动生成电路的输入信号标签名一致！" sqref="F1:M31" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="现态二进制" prompt="由现态十进制列自动计算得到，无需修改" sqref="A2:D31" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3150,15 +3219,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T15" sqref="T15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3524,19 +3593,19 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="str">
         <f>IF(状态转换表!A7=1,状态转换表!A$2&amp;"&amp;",IF(状态转换表!A7=0,"~"&amp;状态转换表!A$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S3&amp;</v>
       </c>
       <c r="B6" s="52" t="str">
         <f>IF(状态转换表!B7=1,状态转换表!B$2&amp;"&amp;",IF(状态转换表!B7=0,"~"&amp;状态转换表!B$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S2&amp;</v>
       </c>
       <c r="C6" s="52" t="str">
         <f>IF(状态转换表!C7=1,状态转换表!C$2&amp;"&amp;",IF(状态转换表!C7=0,"~"&amp;状态转换表!C$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S1&amp;</v>
       </c>
       <c r="D6" s="53" t="str">
         <f>IF(状态转换表!D7=1,状态转换表!D$2&amp;"&amp;",IF(状态转换表!D7=0,"~"&amp;状态转换表!D$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S0&amp;</v>
       </c>
       <c r="E6" s="54" t="str">
         <f>IF(状态转换表!F7&lt;&gt;"",IF(状态转换表!F7=1,状态转换表!F$2&amp;"&amp;",IF(状态转换表!F7=0,"~"&amp;状态转换表!F$2&amp;"&amp;","")),"")</f>
@@ -3544,7 +3613,7 @@
       </c>
       <c r="F6" s="52" t="str">
         <f>IF(状态转换表!G7&lt;&gt;"",IF(状态转换表!G7=1,状态转换表!G$2&amp;"&amp;",IF(状态转换表!G7=0,"~"&amp;状态转换表!G$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>SW&amp;</v>
       </c>
       <c r="G6" s="52" t="str">
         <f>IF(状态转换表!H7&lt;&gt;"",IF(状态转换表!H7=1,状态转换表!H$2&amp;"&amp;",IF(状态转换表!H7=0,"~"&amp;状态转换表!H$2&amp;"&amp;","")),"")</f>
@@ -3572,7 +3641,7 @@
       </c>
       <c r="M6" s="62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;SW</v>
       </c>
       <c r="N6" s="17" t="str">
         <f>IF(状态转换表!O7=1,$M6&amp;"+","")</f>
@@ -3580,7 +3649,7 @@
       </c>
       <c r="O6" s="17" t="str">
         <f>IF(状态转换表!P7=1,$M6&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;SW+</v>
       </c>
       <c r="P6" s="17" t="str">
         <f>IF(状态转换表!Q7=1,$M6&amp;"+","")</f>
@@ -3594,19 +3663,19 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="48" t="str">
         <f>IF(状态转换表!A8=1,状态转换表!A$2&amp;"&amp;",IF(状态转换表!A8=0,"~"&amp;状态转换表!A$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S3&amp;</v>
       </c>
       <c r="B7" s="52" t="str">
         <f>IF(状态转换表!B8=1,状态转换表!B$2&amp;"&amp;",IF(状态转换表!B8=0,"~"&amp;状态转换表!B$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S2&amp;</v>
       </c>
       <c r="C7" s="52" t="str">
         <f>IF(状态转换表!C8=1,状态转换表!C$2&amp;"&amp;",IF(状态转换表!C8=0,"~"&amp;状态转换表!C$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S1&amp;</v>
       </c>
       <c r="D7" s="53" t="str">
         <f>IF(状态转换表!D8=1,状态转换表!D$2&amp;"&amp;",IF(状态转换表!D8=0,"~"&amp;状态转换表!D$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S0&amp;</v>
       </c>
       <c r="E7" s="54" t="str">
         <f>IF(状态转换表!F8&lt;&gt;"",IF(状态转换表!F8=1,状态转换表!F$2&amp;"&amp;",IF(状态转换表!F8=0,"~"&amp;状态转换表!F$2&amp;"&amp;","")),"")</f>
@@ -3618,7 +3687,7 @@
       </c>
       <c r="G7" s="52" t="str">
         <f>IF(状态转换表!H8&lt;&gt;"",IF(状态转换表!H8=1,状态转换表!H$2&amp;"&amp;",IF(状态转换表!H8=0,"~"&amp;状态转换表!H$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>BEQ&amp;</v>
       </c>
       <c r="H7" s="52" t="str">
         <f>IF(状态转换表!I8&lt;&gt;"",IF(状态转换表!I8=1,状态转换表!I$2&amp;"&amp;",IF(状态转换表!I8=0,"~"&amp;状态转换表!I$2&amp;"&amp;","")),"")</f>
@@ -3642,7 +3711,7 @@
       </c>
       <c r="M7" s="62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;BEQ</v>
       </c>
       <c r="N7" s="17" t="str">
         <f>IF(状态转换表!O8=1,$M7&amp;"+","")</f>
@@ -3650,7 +3719,7 @@
       </c>
       <c r="O7" s="17" t="str">
         <f>IF(状态转换表!P8=1,$M7&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;BEQ+</v>
       </c>
       <c r="P7" s="17" t="str">
         <f>IF(状态转换表!Q8=1,$M7&amp;"+","")</f>
@@ -3664,19 +3733,19 @@
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="48" t="str">
         <f>IF(状态转换表!A9=1,状态转换表!A$2&amp;"&amp;",IF(状态转换表!A9=0,"~"&amp;状态转换表!A$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S3&amp;</v>
       </c>
       <c r="B8" s="52" t="str">
         <f>IF(状态转换表!B9=1,状态转换表!B$2&amp;"&amp;",IF(状态转换表!B9=0,"~"&amp;状态转换表!B$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S2&amp;</v>
       </c>
       <c r="C8" s="52" t="str">
         <f>IF(状态转换表!C9=1,状态转换表!C$2&amp;"&amp;",IF(状态转换表!C9=0,"~"&amp;状态转换表!C$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S1&amp;</v>
       </c>
       <c r="D8" s="53" t="str">
         <f>IF(状态转换表!D9=1,状态转换表!D$2&amp;"&amp;",IF(状态转换表!D9=0,"~"&amp;状态转换表!D$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S0&amp;</v>
       </c>
       <c r="E8" s="54" t="str">
         <f>IF(状态转换表!F9&lt;&gt;"",IF(状态转换表!F9=1,状态转换表!F$2&amp;"&amp;",IF(状态转换表!F9=0,"~"&amp;状态转换表!F$2&amp;"&amp;","")),"")</f>
@@ -3712,7 +3781,7 @@
       </c>
       <c r="M8" s="62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>~S3&amp;S2&amp;~S1&amp;~S0</v>
       </c>
       <c r="N8" s="17" t="str">
         <f>IF(状态转换表!O9=1,$M8&amp;"+","")</f>
@@ -3720,7 +3789,7 @@
       </c>
       <c r="O8" s="17" t="str">
         <f>IF(状态转换表!P9=1,$M8&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;S2&amp;~S1&amp;~S0+</v>
       </c>
       <c r="P8" s="17" t="str">
         <f>IF(状态转换表!Q9=1,$M8&amp;"+","")</f>
@@ -3728,25 +3797,25 @@
       </c>
       <c r="Q8" s="17" t="str">
         <f>IF(状态转换表!R9=1,$M8&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;S2&amp;~S1&amp;~S0+</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="str">
         <f>IF(状态转换表!A10=1,状态转换表!A$2&amp;"&amp;",IF(状态转换表!A10=0,"~"&amp;状态转换表!A$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S3&amp;</v>
       </c>
       <c r="B9" s="52" t="str">
         <f>IF(状态转换表!B10=1,状态转换表!B$2&amp;"&amp;",IF(状态转换表!B10=0,"~"&amp;状态转换表!B$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S2&amp;</v>
       </c>
       <c r="C9" s="52" t="str">
         <f>IF(状态转换表!C10=1,状态转换表!C$2&amp;"&amp;",IF(状态转换表!C10=0,"~"&amp;状态转换表!C$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S1&amp;</v>
       </c>
       <c r="D9" s="53" t="str">
         <f>IF(状态转换表!D10=1,状态转换表!D$2&amp;"&amp;",IF(状态转换表!D10=0,"~"&amp;状态转换表!D$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S0&amp;</v>
       </c>
       <c r="E9" s="54" t="str">
         <f>IF(状态转换表!F10&lt;&gt;"",IF(状态转换表!F10=1,状态转换表!F$2&amp;"&amp;",IF(状态转换表!F10=0,"~"&amp;状态转换表!F$2&amp;"&amp;","")),"")</f>
@@ -3782,7 +3851,7 @@
       </c>
       <c r="M9" s="62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>~S3&amp;S2&amp;~S1&amp;S0</v>
       </c>
       <c r="N9" s="17" t="str">
         <f>IF(状态转换表!O10=1,$M9&amp;"+","")</f>
@@ -3790,11 +3859,11 @@
       </c>
       <c r="O9" s="17" t="str">
         <f>IF(状态转换表!P10=1,$M9&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;S2&amp;~S1&amp;S0+</v>
       </c>
       <c r="P9" s="17" t="str">
         <f>IF(状态转换表!Q10=1,$M9&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;S2&amp;~S1&amp;S0+</v>
       </c>
       <c r="Q9" s="17" t="str">
         <f>IF(状态转换表!R10=1,$M9&amp;"+","")</f>
@@ -3804,19 +3873,19 @@
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="str">
         <f>IF(状态转换表!A11=1,状态转换表!A$2&amp;"&amp;",IF(状态转换表!A11=0,"~"&amp;状态转换表!A$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S3&amp;</v>
       </c>
       <c r="B10" s="52" t="str">
         <f>IF(状态转换表!B11=1,状态转换表!B$2&amp;"&amp;",IF(状态转换表!B11=0,"~"&amp;状态转换表!B$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S2&amp;</v>
       </c>
       <c r="C10" s="52" t="str">
         <f>IF(状态转换表!C11=1,状态转换表!C$2&amp;"&amp;",IF(状态转换表!C11=0,"~"&amp;状态转换表!C$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S1&amp;</v>
       </c>
       <c r="D10" s="53" t="str">
         <f>IF(状态转换表!D11=1,状态转换表!D$2&amp;"&amp;",IF(状态转换表!D11=0,"~"&amp;状态转换表!D$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S0&amp;</v>
       </c>
       <c r="E10" s="54" t="str">
         <f>IF(状态转换表!F11&lt;&gt;"",IF(状态转换表!F11=1,状态转换表!F$2&amp;"&amp;",IF(状态转换表!F11=0,"~"&amp;状态转换表!F$2&amp;"&amp;","")),"")</f>
@@ -3836,7 +3905,7 @@
       </c>
       <c r="I10" s="52" t="str">
         <f>IF(状态转换表!J11&lt;&gt;"",IF(状态转换表!J11=1,状态转换表!J$2&amp;"&amp;",IF(状态转换表!J11=0,"~"&amp;状态转换表!J$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>ADDI&amp;</v>
       </c>
       <c r="J10" s="52" t="str">
         <f>IF(状态转换表!K11&lt;&gt;"",IF(状态转换表!K11=1,状态转换表!K$2&amp;"&amp;",IF(状态转换表!K11=0,"~"&amp;状态转换表!K$2&amp;"&amp;","")),"")</f>
@@ -3852,7 +3921,7 @@
       </c>
       <c r="M10" s="62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI</v>
       </c>
       <c r="N10" s="17" t="str">
         <f>IF(状态转换表!O11=1,$M10&amp;"+","")</f>
@@ -3860,11 +3929,11 @@
       </c>
       <c r="O10" s="17" t="str">
         <f>IF(状态转换表!P11=1,$M10&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI+</v>
       </c>
       <c r="P10" s="17" t="str">
         <f>IF(状态转换表!Q11=1,$M10&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI+</v>
       </c>
       <c r="Q10" s="17" t="str">
         <f>IF(状态转换表!R11=1,$M10&amp;"+","")</f>
@@ -3874,19 +3943,19 @@
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="48" t="str">
         <f>IF(状态转换表!A12=1,状态转换表!A$2&amp;"&amp;",IF(状态转换表!A12=0,"~"&amp;状态转换表!A$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S3&amp;</v>
       </c>
       <c r="B11" s="52" t="str">
         <f>IF(状态转换表!B12=1,状态转换表!B$2&amp;"&amp;",IF(状态转换表!B12=0,"~"&amp;状态转换表!B$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S2&amp;</v>
       </c>
       <c r="C11" s="52" t="str">
         <f>IF(状态转换表!C12=1,状态转换表!C$2&amp;"&amp;",IF(状态转换表!C12=0,"~"&amp;状态转换表!C$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S1&amp;</v>
       </c>
       <c r="D11" s="53" t="str">
         <f>IF(状态转换表!D12=1,状态转换表!D$2&amp;"&amp;",IF(状态转换表!D12=0,"~"&amp;状态转换表!D$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S0&amp;</v>
       </c>
       <c r="E11" s="54" t="str">
         <f>IF(状态转换表!F12&lt;&gt;"",IF(状态转换表!F12=1,状态转换表!F$2&amp;"&amp;",IF(状态转换表!F12=0,"~"&amp;状态转换表!F$2&amp;"&amp;","")),"")</f>
@@ -3922,7 +3991,7 @@
       </c>
       <c r="M11" s="62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>~S3&amp;S2&amp;S1&amp;~S0</v>
       </c>
       <c r="N11" s="17" t="str">
         <f>IF(状态转换表!O12=1,$M11&amp;"+","")</f>
@@ -3930,33 +3999,33 @@
       </c>
       <c r="O11" s="17" t="str">
         <f>IF(状态转换表!P12=1,$M11&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;S2&amp;S1&amp;~S0+</v>
       </c>
       <c r="P11" s="17" t="str">
         <f>IF(状态转换表!Q12=1,$M11&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;S2&amp;S1&amp;~S0+</v>
       </c>
       <c r="Q11" s="17" t="str">
         <f>IF(状态转换表!R12=1,$M11&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;S2&amp;S1&amp;~S0+</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="48" t="str">
         <f>IF(状态转换表!A13=1,状态转换表!A$2&amp;"&amp;",IF(状态转换表!A13=0,"~"&amp;状态转换表!A$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S3&amp;</v>
       </c>
       <c r="B12" s="52" t="str">
         <f>IF(状态转换表!B13=1,状态转换表!B$2&amp;"&amp;",IF(状态转换表!B13=0,"~"&amp;状态转换表!B$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S2&amp;</v>
       </c>
       <c r="C12" s="52" t="str">
         <f>IF(状态转换表!C13=1,状态转换表!C$2&amp;"&amp;",IF(状态转换表!C13=0,"~"&amp;状态转换表!C$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S1&amp;</v>
       </c>
       <c r="D12" s="53" t="str">
         <f>IF(状态转换表!D13=1,状态转换表!D$2&amp;"&amp;",IF(状态转换表!D13=0,"~"&amp;状态转换表!D$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S0&amp;</v>
       </c>
       <c r="E12" s="54" t="str">
         <f>IF(状态转换表!F13&lt;&gt;"",IF(状态转换表!F13=1,状态转换表!F$2&amp;"&amp;",IF(状态转换表!F13=0,"~"&amp;状态转换表!F$2&amp;"&amp;","")),"")</f>
@@ -3992,11 +4061,11 @@
       </c>
       <c r="M12" s="62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>~S3&amp;S2&amp;S1&amp;S0</v>
       </c>
       <c r="N12" s="17" t="str">
         <f>IF(状态转换表!O13=1,$M12&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;S2&amp;S1&amp;S0+</v>
       </c>
       <c r="O12" s="17" t="str">
         <f>IF(状态转换表!P13=1,$M12&amp;"+","")</f>
@@ -4014,19 +4083,19 @@
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="48" t="str">
         <f>IF(状态转换表!A14=1,状态转换表!A$2&amp;"&amp;",IF(状态转换表!A14=0,"~"&amp;状态转换表!A$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S3&amp;</v>
       </c>
       <c r="B13" s="52" t="str">
         <f>IF(状态转换表!B14=1,状态转换表!B$2&amp;"&amp;",IF(状态转换表!B14=0,"~"&amp;状态转换表!B$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S2&amp;</v>
       </c>
       <c r="C13" s="52" t="str">
         <f>IF(状态转换表!C14=1,状态转换表!C$2&amp;"&amp;",IF(状态转换表!C14=0,"~"&amp;状态转换表!C$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S1&amp;</v>
       </c>
       <c r="D13" s="53" t="str">
         <f>IF(状态转换表!D14=1,状态转换表!D$2&amp;"&amp;",IF(状态转换表!D14=0,"~"&amp;状态转换表!D$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S0&amp;</v>
       </c>
       <c r="E13" s="54" t="str">
         <f>IF(状态转换表!F14&lt;&gt;"",IF(状态转换表!F14=1,状态转换表!F$2&amp;"&amp;",IF(状态转换表!F14=0,"~"&amp;状态转换表!F$2&amp;"&amp;","")),"")</f>
@@ -4062,7 +4131,7 @@
       </c>
       <c r="M13" s="62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>S3&amp;~S2&amp;~S1&amp;~S0</v>
       </c>
       <c r="N13" s="17" t="str">
         <f>IF(状态转换表!O14=1,$M13&amp;"+","")</f>
@@ -4084,39 +4153,39 @@
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="48" t="str">
         <f>IF(状态转换表!A15=1,状态转换表!A$2&amp;"&amp;",IF(状态转换表!A15=0,"~"&amp;状态转换表!A$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S3&amp;</v>
       </c>
       <c r="B14" s="52" t="str">
         <f>IF(状态转换表!B15=1,状态转换表!B$2&amp;"&amp;",IF(状态转换表!B15=0,"~"&amp;状态转换表!B$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S2&amp;</v>
       </c>
       <c r="C14" s="52" t="str">
         <f>IF(状态转换表!C15=1,状态转换表!C$2&amp;"&amp;",IF(状态转换表!C15=0,"~"&amp;状态转换表!C$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S1&amp;</v>
       </c>
       <c r="D14" s="53" t="str">
         <f>IF(状态转换表!D15=1,状态转换表!D$2&amp;"&amp;",IF(状态转换表!D15=0,"~"&amp;状态转换表!D$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S0&amp;</v>
       </c>
       <c r="E14" s="54" t="str">
         <f>IF(状态转换表!F15&lt;&gt;"",IF(状态转换表!F15=1,状态转换表!F$2&amp;"&amp;",IF(状态转换表!F15=0,"~"&amp;状态转换表!F$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~LW&amp;</v>
       </c>
       <c r="F14" s="52" t="str">
         <f>IF(状态转换表!G15&lt;&gt;"",IF(状态转换表!G15=1,状态转换表!G$2&amp;"&amp;",IF(状态转换表!G15=0,"~"&amp;状态转换表!G$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~SW&amp;</v>
       </c>
       <c r="G14" s="52" t="str">
         <f>IF(状态转换表!H15&lt;&gt;"",IF(状态转换表!H15=1,状态转换表!H$2&amp;"&amp;",IF(状态转换表!H15=0,"~"&amp;状态转换表!H$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~BEQ&amp;</v>
       </c>
       <c r="H14" s="52" t="str">
         <f>IF(状态转换表!I15&lt;&gt;"",IF(状态转换表!I15=1,状态转换表!I$2&amp;"&amp;",IF(状态转换表!I15=0,"~"&amp;状态转换表!I$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~SLT&amp;</v>
       </c>
       <c r="I14" s="52" t="str">
         <f>IF(状态转换表!J15&lt;&gt;"",IF(状态转换表!J15=1,状态转换表!J$2&amp;"&amp;",IF(状态转换表!J15=0,"~"&amp;状态转换表!J$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>~ADDI&amp;</v>
       </c>
       <c r="J14" s="52" t="str">
         <f>IF(状态转换表!K15&lt;&gt;"",IF(状态转换表!K15=1,状态转换表!K$2&amp;"&amp;",IF(状态转换表!K15=0,"~"&amp;状态转换表!K$2&amp;"&amp;","")),"")</f>
@@ -4132,7 +4201,7 @@
       </c>
       <c r="M14" s="62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;~LW&amp;~SW&amp;~BEQ&amp;~SLT&amp;~ADDI</v>
       </c>
       <c r="N14" s="17" t="str">
         <f>IF(状态转换表!O15=1,$M14&amp;"+","")</f>
@@ -4140,11 +4209,11 @@
       </c>
       <c r="O14" s="17" t="str">
         <f>IF(状态转换表!P15=1,$M14&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;~LW&amp;~SW&amp;~BEQ&amp;~SLT&amp;~ADDI+</v>
       </c>
       <c r="P14" s="17" t="str">
         <f>IF(状态转换表!Q15=1,$M14&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;~LW&amp;~SW&amp;~BEQ&amp;~SLT&amp;~ADDI+</v>
       </c>
       <c r="Q14" s="17" t="str">
         <f>IF(状态转换表!R15=1,$M14&amp;"+","")</f>
@@ -4154,19 +4223,19 @@
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="48" t="str">
         <f>IF(状态转换表!A16=1,状态转换表!A$2&amp;"&amp;",IF(状态转换表!A16=0,"~"&amp;状态转换表!A$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S3&amp;</v>
       </c>
       <c r="B15" s="52" t="str">
         <f>IF(状态转换表!B16=1,状态转换表!B$2&amp;"&amp;",IF(状态转换表!B16=0,"~"&amp;状态转换表!B$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>~S2&amp;</v>
       </c>
       <c r="C15" s="52" t="str">
         <f>IF(状态转换表!C16=1,状态转换表!C$2&amp;"&amp;",IF(状态转换表!C16=0,"~"&amp;状态转换表!C$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S1&amp;</v>
       </c>
       <c r="D15" s="53" t="str">
         <f>IF(状态转换表!D16=1,状态转换表!D$2&amp;"&amp;",IF(状态转换表!D16=0,"~"&amp;状态转换表!D$2&amp;"&amp;",""))</f>
-        <v/>
+        <v>S0&amp;</v>
       </c>
       <c r="E15" s="54" t="str">
         <f>IF(状态转换表!F16&lt;&gt;"",IF(状态转换表!F16=1,状态转换表!F$2&amp;"&amp;",IF(状态转换表!F16=0,"~"&amp;状态转换表!F$2&amp;"&amp;","")),"")</f>
@@ -4186,7 +4255,7 @@
       </c>
       <c r="I15" s="52" t="str">
         <f>IF(状态转换表!J16&lt;&gt;"",IF(状态转换表!J16=1,状态转换表!J$2&amp;"&amp;",IF(状态转换表!J16=0,"~"&amp;状态转换表!J$2&amp;"&amp;","")),"")</f>
-        <v/>
+        <v>ADDI&amp;</v>
       </c>
       <c r="J15" s="52" t="str">
         <f>IF(状态转换表!K16&lt;&gt;"",IF(状态转换表!K16=1,状态转换表!K$2&amp;"&amp;",IF(状态转换表!K16=0,"~"&amp;状态转换表!K$2&amp;"&amp;","")),"")</f>
@@ -4202,7 +4271,7 @@
       </c>
       <c r="M15" s="62" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI</v>
       </c>
       <c r="N15" s="17" t="str">
         <f>IF(状态转换表!O16=1,$M15&amp;"+","")</f>
@@ -4210,11 +4279,11 @@
       </c>
       <c r="O15" s="17" t="str">
         <f>IF(状态转换表!P16=1,$M15&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI+</v>
       </c>
       <c r="P15" s="17" t="str">
         <f>IF(状态转换表!Q16=1,$M15&amp;"+","")</f>
-        <v/>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI+</v>
       </c>
       <c r="Q15" s="17" t="str">
         <f>IF(状态转换表!R16=1,$M15&amp;"+","")</f>
@@ -5289,19 +5358,19 @@
       <c r="M31" s="91"/>
       <c r="N31" s="20" t="str">
         <f>IF(LEN(N32)&gt;1,LEFT(N32,LEN(N32)-1),"")</f>
-        <v/>
+        <v>~S3&amp;S2&amp;S1&amp;S0</v>
       </c>
       <c r="O31" s="20" t="str">
         <f>IF(LEN(O32)&gt;1,LEFT(O32,LEN(O32)-1),"")</f>
-        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;LW</v>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;LW+~S3&amp;~S2&amp;S1&amp;S0&amp;SW+~S3&amp;~S2&amp;S1&amp;S0&amp;BEQ+~S3&amp;S2&amp;~S1&amp;~S0+~S3&amp;S2&amp;~S1&amp;S0+~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI+~S3&amp;S2&amp;S1&amp;~S0+~S3&amp;~S2&amp;S1&amp;S0&amp;~LW&amp;~SW&amp;~BEQ&amp;~SLT&amp;~ADDI+~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI</v>
       </c>
       <c r="P31" s="20" t="str">
         <f>IF(LEN(P32)&gt;1,LEFT(P32,LEN(P32)-1),"")</f>
-        <v>~S3&amp;~S2&amp;~S1&amp;S0+~S3&amp;~S2&amp;S1&amp;~S0</v>
+        <v>~S3&amp;~S2&amp;~S1&amp;S0+~S3&amp;~S2&amp;S1&amp;~S0+~S3&amp;S2&amp;~S1&amp;S0+~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI+~S3&amp;S2&amp;S1&amp;~S0+~S3&amp;~S2&amp;S1&amp;S0&amp;~LW&amp;~SW&amp;~BEQ&amp;~SLT&amp;~ADDI+~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI</v>
       </c>
       <c r="Q31" s="22" t="str">
         <f>IF(LEN(Q32)&gt;1,LEFT(Q32,LEN(Q32)-1),"")</f>
-        <v>~S3&amp;~S2&amp;~S1&amp;~S0+~S3&amp;~S2&amp;S1&amp;~S0</v>
+        <v>~S3&amp;~S2&amp;~S1&amp;~S0+~S3&amp;~S2&amp;S1&amp;~S0+~S3&amp;S2&amp;~S1&amp;~S0+~S3&amp;S2&amp;S1&amp;~S0</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5320,19 +5389,19 @@
       <c r="M32" s="64"/>
       <c r="N32" s="21" t="str">
         <f>CONCATENATE(N2,N3,N4,N5,N6,N7,N8,N9,N10,N11,N12,N13,N14,N15,N16,N17,N18,N19,N20,N21,N22,N23,N24,N25,N26,N27,N28,N29,N30)</f>
-        <v/>
+        <v>~S3&amp;S2&amp;S1&amp;S0+</v>
       </c>
       <c r="O32" s="21" t="str">
         <f t="shared" ref="O32:Q32" si="1">CONCATENATE(O2,O3,O4,O5,O6,O7,O8,O9,O10,O11,O12,O13,O14,O15,O16,O17,O18,O19,O20,O21,O22,O23,O24,O25,O26,O27,O28,O29,O30)</f>
-        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;LW+</v>
+        <v>~S3&amp;~S2&amp;S1&amp;S0&amp;LW+~S3&amp;~S2&amp;S1&amp;S0&amp;SW+~S3&amp;~S2&amp;S1&amp;S0&amp;BEQ+~S3&amp;S2&amp;~S1&amp;~S0+~S3&amp;S2&amp;~S1&amp;S0+~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI+~S3&amp;S2&amp;S1&amp;~S0+~S3&amp;~S2&amp;S1&amp;S0&amp;~LW&amp;~SW&amp;~BEQ&amp;~SLT&amp;~ADDI+~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI+</v>
       </c>
       <c r="P32" s="21" t="str">
         <f t="shared" ref="P32" si="2">CONCATENATE(P2,P3,P4,P5,P6,P7,P8,P9,P10,P11,P12,P13,P14,P15,P16,P17,P18,P19,P20,P21,P22,P23,P24,P25,P26,P27,P28,P29,P30)</f>
-        <v>~S3&amp;~S2&amp;~S1&amp;S0+~S3&amp;~S2&amp;S1&amp;~S0+</v>
+        <v>~S3&amp;~S2&amp;~S1&amp;S0+~S3&amp;~S2&amp;S1&amp;~S0+~S3&amp;S2&amp;~S1&amp;S0+~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI+~S3&amp;S2&amp;S1&amp;~S0+~S3&amp;~S2&amp;S1&amp;S0&amp;~LW&amp;~SW&amp;~BEQ&amp;~SLT&amp;~ADDI+~S3&amp;~S2&amp;S1&amp;S0&amp;ADDI+</v>
       </c>
       <c r="Q32" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>~S3&amp;~S2&amp;~S1&amp;~S0+~S3&amp;~S2&amp;S1&amp;~S0+</v>
+        <v>~S3&amp;~S2&amp;~S1&amp;~S0+~S3&amp;~S2&amp;S1&amp;~S0+~S3&amp;S2&amp;~S1&amp;~S0+~S3&amp;S2&amp;S1&amp;~S0+</v>
       </c>
     </row>
     <row r="34" spans="3:15" ht="15" x14ac:dyDescent="0.2">
@@ -5387,9 +5456,9 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态状态位表达式" prompt="次态状态位逻辑表达式，复制到Logisim即可" sqref="N31:Q31"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态状态位" prompt="次态状态位逻辑表达式生成" sqref="Q32:Q34 Q37:Q1048576 N32:P1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态状态位" prompt="次态状态位生成条件最小项" sqref="N1:Q30"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态状态位表达式" prompt="次态状态位逻辑表达式，复制到Logisim即可" sqref="N31:Q31" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态状态位" prompt="次态状态位逻辑表达式生成" sqref="Q32:Q34 Q37:Q1048576 N32:P1048576" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态状态位" prompt="次态状态位生成条件最小项" sqref="N1:Q30" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
@@ -5398,7 +5467,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6454,9 +6523,9 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态机现态二进制" prompt="状态机现态二进制表示，由前列计算得到" sqref="A1:A1048576 B2:C1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态机现态" prompt="状态机现态" sqref="D2:D1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="输出" prompt="输出，只填为1的情况，为零不填" sqref="F2:Q1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态机现态二进制" prompt="状态机现态二进制表示，由前列计算得到" sqref="A1:A1048576 B2:C1048576" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="状态机现态" prompt="状态机现态" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="输出" prompt="输出，只填为1的情况，为零不填" sqref="F2:Q1048576" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6464,7 +6533,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
@@ -8740,10 +8809,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="输出信号产生条件" prompt="输出信号产生条件对应的输入项的最小项" sqref="F1:Q30"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态" prompt="在第一行筛选对应信号为1的条件，最小项列即可包含最终的逻辑表达式" sqref="G37:H38 G40:H1048576 F40:F1048576 F33:F36 F38 I40:I1048576 I38 G33:H35 I33:I35"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="逻辑表达式" prompt="当前列输出信号对应的逻辑表达式，直接复制到Logisim中即可自动生成电路" sqref="F31:Q31"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态状态位" prompt="次态状态位逻辑表达式生成" sqref="F32:Q32 G36"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="输出信号产生条件" prompt="输出信号产生条件对应的输入项的最小项" sqref="F1:Q30" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态" prompt="在第一行筛选对应信号为1的条件，最小项列即可包含最终的逻辑表达式" sqref="G37:H38 G40:H1048576 F40:F1048576 F33:F36 F38 I40:I1048576 I38 G33:H35 I33:I35" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="逻辑表达式" prompt="当前列输出信号对应的逻辑表达式，直接复制到Logisim中即可自动生成电路" sqref="F31:Q31" xr:uid="{00000000-0002-0000-0300-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="次态状态位" prompt="次态状态位逻辑表达式生成" sqref="F32:Q32 G36" xr:uid="{00000000-0002-0000-0300-000003000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>

</xml_diff>